<commit_message>
BD model was added
</commit_message>
<xml_diff>
--- a/Input/Base.xlsx
+++ b/Input/Base.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PCsito\Desktop\GrupLAC-Complete\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\GrupLAC-Complete\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40194F0-5E8A-4BEF-A40C-3DDA0AF1228E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>GrupLAC</t>
   </si>
@@ -57,12 +56,21 @@
   </si>
   <si>
     <t>http://scienti.colciencias.gov.co:8085/gruplac/jsp/visualiza/visualizagr.jsp?nro=00000000002066</t>
+  </si>
+  <si>
+    <t>COL0000001</t>
+  </si>
+  <si>
+    <t>Gruplac de prueba</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8085/gruplac/jsp/visualiza/visualizagr.jsp?nro=00000000019540</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -133,8 +141,8 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Explanatory Text" xfId="1" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Texto explicativo" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -161,7 +169,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -541,14 +549,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.140625" bestFit="1" customWidth="1"/>
@@ -597,8 +605,28 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>123</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>1032456871</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:F1" xr:uid="{3ADA87DC-9D30-48D0-9FA3-D85DC0DC621F}"/>
+  <autoFilter ref="A1:F1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Personal Data was added with CSV and Insert
</commit_message>
<xml_diff>
--- a/Input/Base.xlsx
+++ b/Input/Base.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -134,11 +134,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,6 +626,9 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F4" s="2"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:F1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
clc function was declared
</commit_message>
<xml_diff>
--- a/Input/Base.xlsx
+++ b/Input/Base.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>GrupLAC</t>
   </si>
@@ -65,13 +65,25 @@
   </si>
   <si>
     <t>http://scienti.colciencias.gov.co:8085/gruplac/jsp/visualiza/visualizagr.jsp?nro=00000000019540</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8085/gruplac/jsp/visualiza/visualizagr.jsp?nro=00000000004188</t>
+  </si>
+  <si>
+    <t>asd</t>
+  </si>
+  <si>
+    <t>Grupo de prueba 2</t>
+  </si>
+  <si>
+    <t>http://scienti.colciencias.gov.co:8085/gruplac/jsp/visualiza/visualizagr.jsp?nro=00000000001785</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -89,6 +101,14 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -130,18 +150,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Hipervínculo" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Texto explicativo" xfId="1" builtinId="53" customBuiltin="1"/>
   </cellStyles>
@@ -551,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +613,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>448</v>
       </c>
       <c r="C2" t="s">
@@ -627,11 +650,45 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="F4" s="2"/>
+      <c r="B4">
+        <v>1231</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="2">
+        <v>3123102938</v>
+      </c>
+      <c r="F4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>1231</v>
+      </c>
+      <c r="C5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2">
+        <v>3123102938</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>15</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:F1"/>
+  <hyperlinks>
+    <hyperlink ref="F5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>